<commit_message>
Adding objective IQ functionality
</commit_message>
<xml_diff>
--- a/src/MATLAB/imageInfo.xlsx
+++ b/src/MATLAB/imageInfo.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\212326006\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\prism.nas.gatech.edu\cseng3\vlab\documents\MATLAB\project\GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="5220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Filename</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>IsComposite</t>
+  </si>
+  <si>
+    <t>ParentIndex</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,11 +449,11 @@
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="4" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -464,10 +467,13 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -480,11 +486,14 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -497,11 +506,14 @@
       <c r="D3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -514,11 +526,14 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -531,11 +546,14 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -548,11 +566,14 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -565,11 +586,14 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
@@ -582,11 +606,14 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
@@ -599,11 +626,14 @@
       <c r="D9">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
@@ -616,11 +646,14 @@
       <c r="D10">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -633,11 +666,14 @@
       <c r="D11">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -650,7 +686,10 @@
       <c r="D12">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating subjective IQ run demo settings
</commit_message>
<xml_diff>
--- a/src/MATLAB/imageInfo.xlsx
+++ b/src/MATLAB/imageInfo.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\prism.nas.gatech.edu\cseng3\vlab\documents\MATLAB\project\GUI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\prism.nas.gatech.edu\cseng3\vlab\documents\GitHub\ECE6258\src\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18960" windowHeight="5220"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15165" windowHeight="3345"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Filename</t>
   </si>
@@ -87,6 +87,66 @@
   </si>
   <si>
     <t>ParentIndex</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>20171028_203807.jpg</t>
+  </si>
+  <si>
+    <t>05x07.jpg</t>
+  </si>
+  <si>
+    <t>05x07_2.jpg</t>
+  </si>
+  <si>
+    <t>20161124_144620.jpg</t>
+  </si>
+  <si>
+    <t>revfam1.jpg</t>
+  </si>
+  <si>
+    <t>revfam2.jpg</t>
+  </si>
+  <si>
+    <t>fam_im1.jpg</t>
+  </si>
+  <si>
+    <t>fam1.jpg</t>
+  </si>
+  <si>
+    <t>fam2.jpg</t>
+  </si>
+  <si>
+    <t>fam3.jpg</t>
+  </si>
+  <si>
+    <t>cmh_im1.jpg</t>
+  </si>
+  <si>
+    <t>cmh1.jpg</t>
+  </si>
+  <si>
+    <t>test.jpg</t>
+  </si>
+  <si>
+    <t>test1.jpg</t>
+  </si>
+  <si>
+    <t>test2.jpg</t>
+  </si>
+  <si>
+    <t>famB</t>
+  </si>
+  <si>
+    <t>famA</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -438,11 +498,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -450,7 +508,7 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -693,7 +751,308 @@
         <v>11</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to use only app-generated images
</commit_message>
<xml_diff>
--- a/src/MATLAB/imageInfo.xlsx
+++ b/src/MATLAB/imageInfo.xlsx
@@ -24,54 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Filename</t>
-  </si>
-  <si>
-    <t>im1.jpg</t>
-  </si>
-  <si>
-    <t>im1_c1.jpg</t>
-  </si>
-  <si>
-    <t>im1_c2.jpg</t>
-  </si>
-  <si>
-    <t>im2.jpg</t>
-  </si>
-  <si>
-    <t>im2_c1.jpg</t>
-  </si>
-  <si>
-    <t>im3.jpg</t>
-  </si>
-  <si>
-    <t>im3_c1.jpg</t>
-  </si>
-  <si>
-    <t>im3_c2.jpg</t>
-  </si>
-  <si>
-    <t>im4.jpg</t>
-  </si>
-  <si>
-    <t>im4_c1.jpg</t>
-  </si>
-  <si>
-    <t>im4_c2.jpg</t>
-  </si>
-  <si>
-    <t>One</t>
-  </si>
-  <si>
-    <t>Two</t>
-  </si>
-  <si>
-    <t>Three</t>
-  </si>
-  <si>
-    <t>Four</t>
   </si>
   <si>
     <t>SetIndex</t>
@@ -498,9 +453,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -513,19 +468,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>
@@ -536,7 +491,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -548,7 +503,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -556,7 +511,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -568,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -588,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -596,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -608,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -616,7 +571,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -628,27 +583,27 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -656,19 +611,19 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -676,51 +631,51 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>15</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
@@ -728,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -736,39 +691,39 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -776,19 +731,19 @@
         <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -796,10 +751,10 @@
         <v>5</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -808,247 +763,27 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20">
-        <v>2</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>8</v>
-      </c>
-      <c r="B24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>9</v>
-      </c>
-      <c r="B25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>9</v>
-      </c>
-      <c r="B26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27">
-        <v>3</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>